<commit_message>
Actualización de product y sprint backlog
</commit_message>
<xml_diff>
--- a/Documentacion/Product Backlog.xlsx
+++ b/Documentacion/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugof\OneDrive\Documents\GitHub\Proyecto_App_Inf_2\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E0CEFA-7CAE-4650-B11E-293EF00DFF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2517208B-992D-4B9E-902D-4A85B7424725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,28 @@
     <sheet name="Instructivo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$I$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$I$36</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="113">
   <si>
     <t>Columna</t>
   </si>
@@ -276,33 +289,6 @@
   </si>
   <si>
     <t>Diseñar el esquema de la base de datos según los requisitos del sistema.</t>
-  </si>
-  <si>
-    <t>HT003</t>
-  </si>
-  <si>
-    <t>Como equipo, queremos implementar un sistema de control de versiones (por ejemplo, Git) para gestionar el código fuente y colaborar eficientemente en el desarrollo del proyecto.</t>
-  </si>
-  <si>
-    <t>Implementación de Sistema de Control de Versiones</t>
-  </si>
-  <si>
-    <t>Configurar un repositorio central para el proyecto.</t>
-  </si>
-  <si>
-    <t>Hecho</t>
-  </si>
-  <si>
-    <t>HT004</t>
-  </si>
-  <si>
-    <t>Como arquitectos del sistema, queremos diseñar la arquitectura del sistema para que sea escalable y pueda manejar incrementos en la carga de trabajo.</t>
-  </si>
-  <si>
-    <t>Diseño para Escalabilidad</t>
-  </si>
-  <si>
-    <t>Diseñar la arquitectura del sistema para soportar escalabilidad horizontal y vertical.</t>
   </si>
   <si>
     <t>Sprint 1</t>
@@ -496,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -520,6 +506,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I42"/>
+  <dimension ref="B1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,19 +871,19 @@
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="E5" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>34</v>
@@ -908,19 +895,19 @@
         <v>24</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>112</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>34</v>
@@ -932,19 +919,19 @@
         <v>25</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>34</v>
@@ -956,19 +943,19 @@
         <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="F8" s="5">
         <v>2</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>34</v>
@@ -980,19 +967,19 @@
         <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>34</v>
@@ -1004,19 +991,19 @@
         <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F10" s="5">
         <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>34</v>
@@ -1028,19 +1015,19 @@
         <v>43</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F11" s="5">
         <v>4</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>34</v>
@@ -1061,10 +1048,10 @@
         <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>34</v>
@@ -1085,10 +1072,10 @@
         <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>34</v>
@@ -1109,10 +1096,10 @@
         <v>31</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>34</v>
@@ -1121,28 +1108,28 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -1159,10 +1146,10 @@
         <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>34</v>
@@ -1183,10 +1170,10 @@
         <v>31</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>34</v>
@@ -1207,10 +1194,10 @@
         <v>31</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>34</v>
@@ -1233,10 +1220,10 @@
         <v>31</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>34</v>
@@ -1245,46 +1232,46 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>69</v>
@@ -1305,10 +1292,10 @@
         <v>31</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>34</v>
@@ -1319,181 +1306,173 @@
     </row>
     <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="H23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="I26" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>101</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
@@ -1503,19 +1482,19 @@
     </row>
     <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
@@ -1525,87 +1504,87 @@
     </row>
     <row r="32" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>72</v>
+        <v>89</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>101</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5" t="s">
@@ -1615,19 +1594,19 @@
     </row>
     <row r="36" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5" t="s">
@@ -1635,65 +1614,43 @@
       </c>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+      <c r="I37" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>